<commit_message>
Updated Participant Questionnaire Excel
</commit_message>
<xml_diff>
--- a/Data/Questionnaire/Participants.xlsx
+++ b/Data/Questionnaire/Participants.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inigma/Documents/UZH_Master/Computational_linguistics/QM_in_HCI/our_project/RegressionByEye/Data/Questionnaire/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jangugler/Documents/RegressionByEye/Data/Questionnaire/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476F75DA-2FBE-044B-8F63-000029D8BDEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="18900" windowHeight="11340"/>
+    <workbookView xWindow="9960" yWindow="-20600" windowWidth="18900" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Age</t>
   </si>
@@ -89,12 +90,39 @@
   </si>
   <si>
     <t>P18</t>
+  </si>
+  <si>
+    <t>P09</t>
+  </si>
+  <si>
+    <t>P08</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>P01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,6 +163,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -441,7 +472,7 @@
     <col min="4" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
@@ -485,142 +516,52 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B8">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -629,10 +570,10 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -640,10 +581,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -661,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -670,41 +611,236 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B19">
         <v>29</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <v>0</v>
       </c>
     </row>
@@ -714,7 +850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -726,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added questionnaire info for participants 13 and 14
</commit_message>
<xml_diff>
--- a/Data/Questionnaire/Participants.xlsx
+++ b/Data/Questionnaire/Participants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jangugler/Documents/RegressionByEye/Data/Questionnaire/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twips\Documents\GitHub\RegressionByEye\Data\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476F75DA-2FBE-044B-8F63-000029D8BDEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A9DCEB-D447-49EF-A24C-E9A90F8DF2F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="-20600" windowWidth="18900" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="-20595" windowWidth="18900" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -461,25 +461,25 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -514,37 +514,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -614,12 +614,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -654,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -724,22 +724,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -774,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -809,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -855,7 +915,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -867,7 +927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>